<commit_message>
Created prompt and first sheet
</commit_message>
<xml_diff>
--- a/Top5SA_Travel.xlsx
+++ b/Top5SA_Travel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,19 +446,14 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Highlights</t>
+          <t>Description</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Riverwalk</t>
+          <t>River Walk</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -466,72 +461,67 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.tripadvisor.com/AttractionProductReview-g60956-d11469916-San_Antonio_River_Walk_Cruise_Hop_On_Hop_Off_Trolley_Tour_Tower_of_Americas-San_Ant.html</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">*Hop on or off at any of the bus tour’s 19 stops at your own leisure *Cruise down the San Antonio River Walk on a boat *Includes 4-D theater ride at the Tower of the Americas    </t>
+          <t xml:space="preserve">See San Antonio three ways with this combination bus, boat, and viewing tower experience. </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>The Alamo</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+          <t>Missons Heritage Tour</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Consists of five missions filled with history and religious importance.</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Missions National Historical Park</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+          <t>Haunted History Ghost Tour</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tour some of the most haunted sites in the city at night.</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Natural Bridge Caverns</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+          <t>San Antonio Zoo</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Home to thousands of exotic animals, the zoo is a guaranteed hit with people of all ages. </t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Pear District</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Haunted History Ghost Tour</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://www.tripadvisor.com/AttractionProductReview-g60956-d11456681-San_Antonio_Haunted_History_Ghost_Tour-San_Antonio_Texas.html </t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>*Hear tales of haunting and paranormal activity in Texas *A costumed guide leads the way by lantern—for an extra scare factor *Convenient and easy-to-find meeting spot</t>
+          <t>Segway Tour</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cruise through San Antonio on a 2-hour Segway tour that takes in the highlights of historic downtown</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
End of day updates
</commit_message>
<xml_diff>
--- a/Top5SA_Travel.xlsx
+++ b/Top5SA_Travel.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tour three ways with bus, boat, and tower experience. </t>
+          <t xml:space="preserve">See San Antonio three ways with this combination bus, boat, and viewing tower experience. </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Five missions filled with history and religious importance.</t>
+          <t>Visit five missions filled with history and religious importance.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Tour some of the most haunted sites in the city at night.</t>
+          <t xml:space="preserve">Tour some of the most haunted sites in the city at night. Guide leads the way by lantern as you hear about the paranormal activity. </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Thousands of exotic animals, guaranteed hit with people of all ages. </t>
+          <t xml:space="preserve">Home to thousands of exotic animals, guaranteed hit with people of all ages. </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2-hour Segway tour that takes in the highlights of historic downtown.</t>
+          <t>Cruise through San Antonio on a 2-hour Segway tour that takes in the highlights of historic downtown.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">

</xml_diff>